<commit_message>
Oh yeah on top of the game now baybee
</commit_message>
<xml_diff>
--- a/PChemLab/Lab 3.xlsx
+++ b/PChemLab/Lab 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\repos\Courses-Fall2022\PChemLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21163CD2-C1FE-4A42-9E04-66D445B27782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F9A7D1-A2B8-457B-91E4-EC788D1FDF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="1575" windowWidth="17100" windowHeight="10260" activeTab="1" xr2:uid="{EFE65110-107A-44E6-9116-D3E3FC84E6F0}"/>
+    <workbookView xWindow="11700" yWindow="1485" windowWidth="17100" windowHeight="10260" xr2:uid="{EFE65110-107A-44E6-9116-D3E3FC84E6F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88965B1D-CC53-48FB-BF04-D278D673D193}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FC4062-6F78-49AD-9A1E-21844A31E752}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,15 +1412,15 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>75.3</v>
+        <v>-75.3</v>
       </c>
       <c r="C2">
-        <f>A2+1</f>
+        <f t="shared" ref="C2:C43" si="0">A2+1</f>
         <v>3</v>
       </c>
       <c r="D2">
-        <f>B2+273.15</f>
-        <v>348.45</v>
+        <f t="shared" ref="D2:D43" si="1">B2+273.15</f>
+        <v>197.84999999999997</v>
       </c>
       <c r="E2">
         <f>LOG(C2,2.71828182846)</f>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="F2">
         <f>1/D2</f>
-        <v>2.8698522026115655E-3</v>
+        <v>5.0543340914834482E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1436,23 +1436,23 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>74.5</v>
+        <v>-74.5</v>
       </c>
       <c r="C3">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D3">
-        <f>B3+273.15</f>
-        <v>347.65</v>
+        <f t="shared" si="1"/>
+        <v>198.64999999999998</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E43" si="0">LOG(C3,2.71828182846)</f>
+        <f t="shared" ref="E3:E43" si="2">LOG(C3,2.71828182846)</f>
         <v>1.609437912433535</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F43" si="1">1/D3</f>
-        <v>2.8764562059542644E-3</v>
+        <f t="shared" ref="F3:F43" si="3">1/D3</f>
+        <v>5.033979360684622E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,23 +1460,23 @@
         <v>5.5</v>
       </c>
       <c r="B4">
-        <v>73.5</v>
+        <v>-73.5</v>
       </c>
       <c r="C4">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="D4">
-        <f>B4+273.15</f>
-        <v>346.65</v>
+        <f t="shared" si="1"/>
+        <v>199.64999999999998</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.8718021769009339</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>2.8847540747151306E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.0087653393438526E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1484,23 +1484,23 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>72.599999999999994</v>
+        <v>-72.599999999999994</v>
       </c>
       <c r="C5">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D5">
-        <f>B5+273.15</f>
-        <v>345.75</v>
+        <f t="shared" si="1"/>
+        <v>200.54999999999998</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0794415416791052</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>2.8922631959508315E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.9862877088007983E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1508,23 +1508,23 @@
         <v>8.5</v>
       </c>
       <c r="B6">
-        <v>71.7</v>
+        <v>-71.7</v>
       </c>
       <c r="C6">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="D6">
-        <f>B6+273.15</f>
-        <v>344.84999999999997</v>
+        <f t="shared" si="1"/>
+        <v>201.45</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2512917986057044</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>2.8998115122517041E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.964010920824026E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,23 +1532,23 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>70.900000000000006</v>
+        <v>-70.900000000000006</v>
       </c>
       <c r="C7">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="D7">
-        <f>B7+273.15</f>
-        <v>344.04999999999995</v>
+        <f t="shared" si="1"/>
+        <v>202.24999999999997</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3978952727975282</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>2.9065542799011778E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.9443757725587149E-3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1556,23 +1556,23 @@
         <v>11.5</v>
       </c>
       <c r="B8">
-        <v>70.3</v>
+        <v>-70.3</v>
       </c>
       <c r="C8">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="D8">
-        <f>B8+273.15</f>
-        <v>343.45</v>
+        <f t="shared" si="1"/>
+        <v>202.84999999999997</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5257286443073683</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>2.9116319697190278E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.9297510475720986E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1580,23 +1580,23 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>69.400000000000006</v>
+        <v>-69.400000000000006</v>
       </c>
       <c r="C9">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="D9">
-        <f>B9+273.15</f>
-        <v>342.54999999999995</v>
+        <f t="shared" si="1"/>
+        <v>203.74999999999997</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.6390573296143316</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
-        <v>2.9192818566632613E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.9079754601226997E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1604,23 +1604,23 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>68.900000000000006</v>
+        <v>-68.900000000000006</v>
       </c>
       <c r="C10">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D10">
-        <f>B10+273.15</f>
-        <v>342.04999999999995</v>
+        <f t="shared" si="1"/>
+        <v>204.24999999999997</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7080502011012588</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
-        <v>2.9235491887151005E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8959608323133419E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1628,23 +1628,23 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>68.2</v>
+        <v>-68.2</v>
       </c>
       <c r="C11">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D11">
-        <f>B11+273.15</f>
-        <v>341.34999999999997</v>
+        <f t="shared" si="1"/>
+        <v>204.95</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.833213344055221</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
-        <v>2.9295444558371177E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8792388387411565E-3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1652,23 +1652,23 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>67.599999999999994</v>
+        <v>-67.599999999999994</v>
       </c>
       <c r="C12">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D12">
-        <f>B12+273.15</f>
-        <v>340.75</v>
+        <f t="shared" si="1"/>
+        <v>205.54999999999998</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.8903717578951493</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
-        <v>2.93470286133529E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8649963512527369E-3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1676,23 +1676,23 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>67.099999999999994</v>
+        <v>-67.099999999999994</v>
       </c>
       <c r="C13">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="D13">
-        <f>B13+273.15</f>
-        <v>340.25</v>
+        <f t="shared" si="1"/>
+        <v>206.04999999999998</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.944438979165406</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>2.9390154298310064E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8531909730647905E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1700,23 +1700,23 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>66.5</v>
+        <v>-66.5</v>
       </c>
       <c r="C14">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="D14">
-        <f>B14+273.15</f>
-        <v>339.65</v>
+        <f t="shared" si="1"/>
+        <v>206.64999999999998</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.0445224377223536</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
-        <v>2.9442072721919624E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8390999274135014E-3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1724,23 +1724,23 @@
         <v>21.5</v>
       </c>
       <c r="B15">
-        <v>66</v>
+        <v>-66</v>
       </c>
       <c r="C15">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
       <c r="D15">
-        <f>B15+273.15</f>
-        <v>339.15</v>
+        <f t="shared" si="1"/>
+        <v>207.14999999999998</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1135153092092804</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
-        <v>2.9485478401887074E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8274197441467541E-3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1748,23 +1748,23 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>65.400000000000006</v>
+        <v>-65.400000000000006</v>
       </c>
       <c r="C16">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="D16">
-        <f>B16+273.15</f>
-        <v>338.54999999999995</v>
+        <f t="shared" si="1"/>
+        <v>207.74999999999997</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1780538303468293</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>2.9537734455767246E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8134777376654643E-3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1772,23 +1772,23 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>64.900000000000006</v>
+        <v>-64.900000000000006</v>
       </c>
       <c r="C17">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D17">
-        <f>B17+273.15</f>
-        <v>338.04999999999995</v>
+        <f t="shared" si="1"/>
+        <v>208.24999999999997</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2188758248670699</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
-        <v>2.958142286643988E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.8019207683073235E-3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1796,23 +1796,23 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>64.400000000000006</v>
+        <v>-64.400000000000006</v>
       </c>
       <c r="C18">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="D18">
-        <f>B18+273.15</f>
-        <v>337.54999999999995</v>
+        <f t="shared" si="1"/>
+        <v>208.74999999999997</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2958368660031714</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
-        <v>2.9625240705080731E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7904191616766475E-3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,23 +1820,23 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>64</v>
+        <v>-64</v>
       </c>
       <c r="C19">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="D19">
-        <f>B19+273.15</f>
-        <v>337.15</v>
+        <f t="shared" si="1"/>
+        <v>209.14999999999998</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.3322045101740332</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
-        <v>2.9660388551090021E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7812574707147984E-3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1844,23 +1844,23 @@
         <v>28.5</v>
       </c>
       <c r="B20">
-        <v>63.5</v>
+        <v>-63.5</v>
       </c>
       <c r="C20">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>29.5</v>
       </c>
       <c r="D20">
-        <f>B20+273.15</f>
-        <v>336.65</v>
+        <f t="shared" si="1"/>
+        <v>209.64999999999998</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.3843902633445855</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
-        <v>2.9704440813901681E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7698545194371578E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,23 +1868,23 @@
         <v>30</v>
       </c>
       <c r="B21">
-        <v>63</v>
+        <v>-63</v>
       </c>
       <c r="C21">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="D21">
-        <f>B21+273.15</f>
-        <v>336.15</v>
+        <f t="shared" si="1"/>
+        <v>210.14999999999998</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.4339872044839401</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
-        <v>2.974862412613417E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7585058291696415E-3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1892,23 +1892,23 @@
         <v>31</v>
       </c>
       <c r="B22">
-        <v>62.5</v>
+        <v>-62.5</v>
       </c>
       <c r="C22">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="D22">
-        <f>B22+273.15</f>
-        <v>335.65</v>
+        <f t="shared" si="1"/>
+        <v>210.64999999999998</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.4657359027985093</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
-        <v>2.9792939073439596E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7472110135295519E-3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1916,23 +1916,23 @@
         <v>33</v>
       </c>
       <c r="B23">
-        <v>62.1</v>
+        <v>-62.1</v>
       </c>
       <c r="C23">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="D23">
-        <f>B23+273.15</f>
-        <v>335.25</v>
+        <f t="shared" si="1"/>
+        <v>211.04999999999998</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.526360524614923</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
-        <v>2.9828486204325128E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7382136934375745E-3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1940,23 +1940,23 @@
         <v>34.5</v>
       </c>
       <c r="B24">
-        <v>61.7</v>
+        <v>-61.7</v>
       </c>
       <c r="C24">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
         <v>35.5</v>
       </c>
       <c r="D24">
-        <f>B24+273.15</f>
-        <v>334.84999999999997</v>
+        <f t="shared" si="1"/>
+        <v>211.45</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.569532696480116</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
-        <v>2.9864118261908319E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7292504138094112E-3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1964,23 +1964,23 @@
         <v>36</v>
       </c>
       <c r="B25">
-        <v>61.2</v>
+        <v>-61.2</v>
       </c>
       <c r="C25">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="D25">
-        <f>B25+273.15</f>
-        <v>334.34999999999997</v>
+        <f t="shared" si="1"/>
+        <v>211.95</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.610917912642956</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
-        <v>2.9908778226409452E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7180938900684127E-3</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1988,23 +1988,23 @@
         <v>37</v>
       </c>
       <c r="B26">
-        <v>60.7</v>
+        <v>-60.7</v>
       </c>
       <c r="C26">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="D26">
-        <f>B26+273.15</f>
-        <v>333.84999999999997</v>
+        <f t="shared" si="1"/>
+        <v>212.45</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.637586159725108</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
-        <v>2.9953571963456647E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7069898799717586E-3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,23 +2012,23 @@
         <v>39</v>
       </c>
       <c r="B27">
-        <v>60.4</v>
+        <v>-60.4</v>
       </c>
       <c r="C27">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="D27">
-        <f>B27+273.15</f>
-        <v>333.54999999999995</v>
+        <f t="shared" si="1"/>
+        <v>212.74999999999997</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6888794541126404</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
-        <v>2.9980512666766606E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.7003525264394837E-3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2036,23 +2036,23 @@
         <v>40.5</v>
       </c>
       <c r="B28">
-        <v>60</v>
+        <v>-60</v>
       </c>
       <c r="C28">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>41.5</v>
       </c>
       <c r="D28">
-        <f>B28+273.15</f>
-        <v>333.15</v>
+        <f t="shared" si="1"/>
+        <v>213.14999999999998</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7256934272353437</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
-        <v>3.0016509079993999E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6915317851278443E-3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2060,23 +2060,23 @@
         <v>42</v>
       </c>
       <c r="B29">
-        <v>59.7</v>
+        <v>-59.7</v>
       </c>
       <c r="C29">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="D29">
-        <f>B29+273.15</f>
-        <v>332.84999999999997</v>
+        <f t="shared" si="1"/>
+        <v>213.45</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7612001156922412</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
-        <v>3.0043563166591561E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6849379245724994E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2084,23 +2084,23 @@
         <v>44</v>
       </c>
       <c r="B30">
-        <v>59.3</v>
+        <v>-59.3</v>
       </c>
       <c r="C30">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="D30">
-        <f>B30+273.15</f>
-        <v>332.45</v>
+        <f t="shared" si="1"/>
+        <v>213.84999999999997</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8066624897689825</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
-        <v>3.0079711234772149E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6761748889408471E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2108,23 +2108,23 @@
         <v>45</v>
       </c>
       <c r="B31">
-        <v>59.1</v>
+        <v>-59.1</v>
       </c>
       <c r="C31">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="D31">
-        <f>B31+273.15</f>
-        <v>332.25</v>
+        <f t="shared" si="1"/>
+        <v>214.04999999999998</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8286413964877504</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
-        <v>3.0097817908201654E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6718056528848402E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2132,23 +2132,23 @@
         <v>47</v>
       </c>
       <c r="B32">
-        <v>58.6</v>
+        <v>-58.6</v>
       </c>
       <c r="C32">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="D32">
-        <f>B32+273.15</f>
-        <v>331.75</v>
+        <f t="shared" si="1"/>
+        <v>214.54999999999998</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8712010109065313</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
-        <v>3.0143180105501131E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6609182008855747E-3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2156,23 +2156,23 @@
         <v>49</v>
       </c>
       <c r="B33">
-        <v>58.3</v>
+        <v>-58.3</v>
       </c>
       <c r="C33">
-        <f>A33+1</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="D33">
-        <f>B33+273.15</f>
-        <v>331.45</v>
+        <f t="shared" si="1"/>
+        <v>214.84999999999997</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.9120230054267719</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
-        <v>3.017046311660884E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6544100535257163E-3</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2180,23 +2180,23 @@
         <v>50</v>
       </c>
       <c r="B34">
-        <v>57.9</v>
+        <v>-57.9</v>
       </c>
       <c r="C34">
-        <f>A34+1</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="D34">
-        <f>B34+273.15</f>
-        <v>331.04999999999995</v>
+        <f t="shared" si="1"/>
+        <v>215.24999999999997</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.9318256327229446</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
-        <v>3.0206917384080958E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6457607433217198E-3</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2204,23 +2204,23 @@
         <v>52</v>
       </c>
       <c r="B35">
-        <v>57.6</v>
+        <v>-57.6</v>
       </c>
       <c r="C35">
-        <f>A35+1</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="D35">
-        <f>B35+273.15</f>
-        <v>330.75</v>
+        <f t="shared" si="1"/>
+        <v>215.54999999999998</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.9702919135507271</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
-        <v>3.0234315948601664E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6392948271862678E-3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,23 +2228,23 @@
         <v>53</v>
       </c>
       <c r="B36">
-        <v>57.2</v>
+        <v>-57.2</v>
       </c>
       <c r="C36">
-        <f>A36+1</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="D36">
-        <f>B36+273.15</f>
-        <v>330.34999999999997</v>
+        <f t="shared" si="1"/>
+        <v>215.95</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.9889840465628734</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
-        <v>3.0270924776751931E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6307015512850203E-3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2252,23 +2252,23 @@
         <v>55</v>
       </c>
       <c r="B37">
-        <v>56.9</v>
+        <v>-56.9</v>
       </c>
       <c r="C37">
-        <f>A37+1</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="D37">
-        <f>B37+273.15</f>
-        <v>330.04999999999995</v>
+        <f t="shared" si="1"/>
+        <v>216.24999999999997</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.0253516907337357</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
-        <v>3.029843963035904E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6242774566473991E-3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2276,23 +2276,23 @@
         <v>57</v>
       </c>
       <c r="B38">
-        <v>56.4</v>
+        <v>-56.4</v>
       </c>
       <c r="C38">
-        <f>A38+1</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="D38">
-        <f>B38+273.15</f>
-        <v>329.54999999999995</v>
+        <f t="shared" si="1"/>
+        <v>216.74999999999997</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.0604430105449927</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
-        <v>3.0344409042633901E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6136101499423309E-3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2300,23 +2300,23 @@
         <v>59</v>
       </c>
       <c r="B39">
-        <v>56.1</v>
+        <v>-56.1</v>
       </c>
       <c r="C39">
-        <f>A39+1</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="D39">
-        <f>B39+273.15</f>
-        <v>329.25</v>
+        <f t="shared" si="1"/>
+        <v>217.04999999999998</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.0943445622206625</v>
       </c>
       <c r="F39">
-        <f t="shared" si="1"/>
-        <v>3.0372057706909645E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6072333563695004E-3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2324,23 +2324,23 @@
         <v>59.5</v>
       </c>
       <c r="B40">
-        <v>56.3</v>
+        <v>-56.3</v>
       </c>
       <c r="C40">
-        <f>A40+1</f>
+        <f t="shared" si="0"/>
         <v>60.5</v>
       </c>
       <c r="D40">
-        <f>B40+273.15</f>
-        <v>329.45</v>
+        <f t="shared" si="1"/>
+        <v>216.84999999999997</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.1026433650353544</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
-        <v>3.0353619669145548E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.611482591653217E-3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,23 +2348,23 @@
         <v>60</v>
       </c>
       <c r="B41">
-        <v>56.4</v>
+        <v>-56.4</v>
       </c>
       <c r="C41">
-        <f>A41+1</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="D41">
-        <f>B41+273.15</f>
-        <v>329.54999999999995</v>
+        <f t="shared" si="1"/>
+        <v>216.74999999999997</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.1108738641718672</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
-        <v>3.0344409042633901E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6136101499423309E-3</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2372,23 +2372,23 @@
         <v>60.5</v>
       </c>
       <c r="B42">
-        <v>56.3</v>
+        <v>-56.3</v>
       </c>
       <c r="C42">
-        <f>A42+1</f>
+        <f t="shared" si="0"/>
         <v>61.5</v>
       </c>
       <c r="D42">
-        <f>B42+273.15</f>
-        <v>329.45</v>
+        <f t="shared" si="1"/>
+        <v>216.84999999999997</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.1190371748110257</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
-        <v>3.0353619669145548E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.611482591653217E-3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2396,23 +2396,23 @@
         <v>60.5</v>
       </c>
       <c r="B43">
-        <v>56.5</v>
+        <v>-56.5</v>
       </c>
       <c r="C43">
-        <f>A43+1</f>
+        <f t="shared" si="0"/>
         <v>61.5</v>
       </c>
       <c r="D43">
-        <f>B43+273.15</f>
-        <v>329.65</v>
+        <f t="shared" si="1"/>
+        <v>216.64999999999998</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.1190371748110257</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
-        <v>3.033520400424693E-3</v>
+        <f t="shared" si="3"/>
+        <v>4.6157396722824838E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>